<commit_message>
add find and confirm max tests
</commit_message>
<xml_diff>
--- a/Документы/Профиль_нагрузки.xlsx
+++ b/Документы/Профиль_нагрузки.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LoadRunner\LRProjects\Скрипты\Документы\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ed230\OneDrive\Рабочий стол\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCECDFD-4457-4AC5-84CF-2C88DAFE7EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3B3CB15-B7C2-4DE4-ABF6-ED8783DBEEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Автоматизированный расчет" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="108" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -223,7 +223,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="102">
   <si>
     <t>Вход в систему</t>
   </si>
@@ -471,9 +471,6 @@
     <t>Duration + Think_time</t>
   </si>
   <si>
-    <t>Action_Transaction</t>
-  </si>
-  <si>
     <t>Профиль</t>
   </si>
   <si>
@@ -523,9 +520,6 @@
   </si>
   <si>
     <t>UC5_BuyTicket</t>
-  </si>
-  <si>
-    <t>vuser_init_Transaction</t>
   </si>
   <si>
     <t>FALSE</t>
@@ -1099,7 +1093,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -1501,15 +1495,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FFDEE2E6"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1594,7 +1579,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1742,9 +1727,19 @@
     <xf numFmtId="2" fontId="0" fillId="45" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="66" applyBorder="1"/>
     <xf numFmtId="0" fontId="34" fillId="46" borderId="2" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1761,25 +1756,12 @@
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="47" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="34" fillId="46" borderId="33" xfId="80" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="46" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="66" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="46" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="2" fontId="33" fillId="46" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="81">
@@ -1865,216 +1847,27 @@
     <cellStyle name="Текст предупреждения" xfId="15" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Хороший" xfId="1" builtinId="26" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="70">
+  <dxfs count="7">
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.00000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2087,971 +1880,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3077" name="AutoShape 5">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B7FA54C-6071-3675-BB21-7EA8E61ADB4B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="952500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3078" name="AutoShape 6">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AD9021F-AB03-BDC7-D3C8-0DE69D4EC523}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1143000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3079" name="AutoShape 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7759D7D-27A6-C2A4-3597-36BB1D976DDB}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1333500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3080" name="AutoShape 8">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D6E6BFD-9A25-653A-0135-7C398146FCEA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1524000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3081" name="AutoShape 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22A03088-9EFB-B148-07A2-81EBDD576C2D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1714500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3082" name="AutoShape 10">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4FC3DBB-5F73-C168-F2B3-D0625A3F1D9D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1905000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3083" name="AutoShape 11">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65D9C5B0-2BE7-C39A-75FC-9215133DACFC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="2095500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3084" name="AutoShape 12">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C520393C-6AEA-3641-9BA6-7B5A110620CC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="2286000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>121920</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3093" name="AutoShape 21">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAC5F597-EAB9-27EB-B7EC-DB069D795E5C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="3992880"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3099" name="AutoShape 27">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3CA98EB-0BBE-63E3-9D97-83F52AADE5CC}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1143000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3100" name="AutoShape 28">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAF17A18-C04F-7AE0-B5BF-3E8D707D59F7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1333500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3101" name="AutoShape 29">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F71B87FB-882C-84E3-0F9E-2D1F98489BA0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1524000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3102" name="AutoShape 30">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDE38975-3ED0-AADD-E420-DD3F6B9D740F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1714500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3103" name="AutoShape 31">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{433EB5B6-E7A4-A38C-9CE4-03C5D8A4269F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1905000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3104" name="AutoShape 32">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAC7FC2F-0B95-CE53-5D9D-51DB3B96F0C7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="2095500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3105" name="AutoShape 33">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34801691-ECD9-E909-C65E-5B8EFA492BA5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="2286000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3120" name="AutoShape 48">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CCC336DE-121C-85D2-44DD-6AE86B20188F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1333500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3121" name="AutoShape 49">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDA4ADC2-2B80-A37F-3C60-7D738A41E6C2}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1524000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3123" name="AutoShape 51">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6CEF4F-655F-1E4B-426D-0942264286DD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="1905000"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3124" name="AutoShape 52">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86C0DB69-A25F-CE8B-A658-96EA3588515F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="2499360" y="2095500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3443,7 +2271,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="Сводная таблица2" cacheId="108" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="Сводная таблица2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Значения" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="I1:J14" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField showAll="0"/>
@@ -3523,25 +2351,25 @@
     <dataField name="Сумма по полю Итого" fld="7" baseField="0" baseItem="0" numFmtId="1"/>
   </dataFields>
   <formats count="7">
-    <format dxfId="28">
+    <format dxfId="6">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="5">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="4">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="3">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="32">
+    <format dxfId="2">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="1">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="34">
+    <format dxfId="0">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -3822,7 +2650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
@@ -3902,7 +2730,7 @@
         <v>49</v>
       </c>
       <c r="T1" s="57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U1" s="47" t="s">
         <v>47</v>
@@ -4313,16 +3141,16 @@
       <c r="J7" s="17">
         <v>23.076923076923073</v>
       </c>
-      <c r="M7" s="110" t="s">
+      <c r="M7" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="113">
+      <c r="N7" s="104">
         <v>4</v>
       </c>
-      <c r="O7" s="114">
+      <c r="O7" s="105">
         <v>15</v>
       </c>
-      <c r="P7" s="111">
+      <c r="P7" s="36">
         <f t="shared" si="3"/>
         <v>19</v>
       </c>
@@ -4332,7 +3160,7 @@
       <c r="R7" s="44">
         <v>1</v>
       </c>
-      <c r="S7" s="112">
+      <c r="S7" s="45">
         <f t="shared" si="2"/>
         <v>0.1111111111111111</v>
       </c>
@@ -4359,23 +3187,23 @@
       <c r="C8" s="22">
         <v>1</v>
       </c>
-      <c r="D8" s="108">
+      <c r="D8" s="102">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E8" s="105">
+      <c r="E8" s="99">
         <f t="shared" si="7"/>
         <v>52</v>
       </c>
-      <c r="F8" s="106">
+      <c r="F8" s="100">
         <f t="shared" si="0"/>
         <v>1.1538461538461537</v>
       </c>
-      <c r="G8" s="107">
+      <c r="G8" s="101">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H8" s="105">
+      <c r="H8" s="99">
         <f t="shared" si="8"/>
         <v>23.076923076923073</v>
       </c>
@@ -4410,23 +3238,23 @@
       <c r="C9" s="22">
         <v>1</v>
       </c>
-      <c r="D9" s="104">
+      <c r="D9" s="98">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E9" s="105">
+      <c r="E9" s="99">
         <f t="shared" si="7"/>
         <v>52</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="100">
         <f t="shared" si="0"/>
         <v>1.1538461538461537</v>
       </c>
-      <c r="G9" s="107">
+      <c r="G9" s="101">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H9" s="105">
+      <c r="H9" s="99">
         <f t="shared" si="8"/>
         <v>23.076923076923073</v>
       </c>
@@ -4447,23 +3275,23 @@
       <c r="C10" s="22">
         <v>1</v>
       </c>
-      <c r="D10" s="104">
+      <c r="D10" s="98">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E10" s="105">
+      <c r="E10" s="99">
         <f t="shared" si="7"/>
         <v>52</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="100">
         <f t="shared" si="0"/>
         <v>1.1538461538461537</v>
       </c>
-      <c r="G10" s="107">
+      <c r="G10" s="101">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H10" s="105">
+      <c r="H10" s="99">
         <f t="shared" si="8"/>
         <v>23.076923076923073</v>
       </c>
@@ -4484,23 +3312,23 @@
       <c r="C11" s="22">
         <v>1</v>
       </c>
-      <c r="D11" s="104">
+      <c r="D11" s="98">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E11" s="105">
+      <c r="E11" s="99">
         <f t="shared" si="7"/>
         <v>52</v>
       </c>
-      <c r="F11" s="106">
+      <c r="F11" s="100">
         <f t="shared" si="0"/>
         <v>1.1538461538461537</v>
       </c>
-      <c r="G11" s="107">
+      <c r="G11" s="101">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H11" s="105">
+      <c r="H11" s="99">
         <f t="shared" si="8"/>
         <v>23.076923076923073</v>
       </c>
@@ -4521,23 +3349,23 @@
       <c r="C12" s="22">
         <v>1</v>
       </c>
-      <c r="D12" s="109">
+      <c r="D12" s="103">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="E12" s="105">
+      <c r="E12" s="99">
         <f t="shared" si="7"/>
         <v>52</v>
       </c>
-      <c r="F12" s="106">
+      <c r="F12" s="100">
         <f t="shared" si="0"/>
         <v>1.1538461538461537</v>
       </c>
-      <c r="G12" s="107">
+      <c r="G12" s="101">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H12" s="105">
+      <c r="H12" s="99">
         <f t="shared" si="8"/>
         <v>23.076923076923073</v>
       </c>
@@ -5244,14 +4072,14 @@
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="99" t="s">
+      <c r="A38" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="100"/>
-      <c r="C38" s="101" t="s">
-        <v>83</v>
-      </c>
-      <c r="D38" s="102"/>
+      <c r="B38" s="108"/>
+      <c r="C38" s="109" t="s">
+        <v>82</v>
+      </c>
+      <c r="D38" s="110"/>
     </row>
     <row r="39" spans="1:9" ht="72" x14ac:dyDescent="0.35">
       <c r="A39" s="25" t="s">
@@ -5306,11 +4134,11 @@
       </c>
       <c r="H40" s="22">
         <f>VLOOKUP(F40,SummaryReport!A:J,8,FALSE)</f>
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I40" s="20">
         <f t="shared" ref="I40:I51" si="20">1-G40/H40</f>
-        <v>4.5366398307574829E-2</v>
+        <v>4.0233959588798385E-2</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="18" x14ac:dyDescent="0.3">
@@ -5372,11 +4200,11 @@
       </c>
       <c r="H42" s="22">
         <f>VLOOKUP(F42,SummaryReport!A:J,8,FALSE)</f>
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="I42" s="20">
         <f t="shared" si="20"/>
-        <v>6.8501591866078071E-2</v>
+        <v>2.2839905192846621E-2</v>
       </c>
     </row>
     <row r="43" spans="1:9" ht="36" x14ac:dyDescent="0.3">
@@ -5405,11 +4233,11 @@
       </c>
       <c r="H43" s="22">
         <f>VLOOKUP(F43,SummaryReport!A:J,8,FALSE)</f>
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I43" s="20">
         <f t="shared" si="20"/>
-        <v>1.4611761864509298E-2</v>
+        <v>-1.8981018981018671E-2</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="18" x14ac:dyDescent="0.3">
@@ -5438,11 +4266,11 @@
       </c>
       <c r="H44" s="22">
         <f>VLOOKUP(F44,SummaryReport!A:J,8,FALSE)</f>
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I44" s="20">
         <f t="shared" si="20"/>
-        <v>1.4611761864509298E-2</v>
+        <v>-1.8981018981018671E-2</v>
       </c>
     </row>
     <row r="45" spans="1:9" ht="18" x14ac:dyDescent="0.3">
@@ -5504,11 +4332,11 @@
       </c>
       <c r="H46" s="22">
         <f>VLOOKUP(F46,SummaryReport!A:J,8,FALSE)</f>
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I46" s="20">
         <f t="shared" si="20"/>
-        <v>1.7286084701814142E-3</v>
+        <v>-9.6153846153848033E-3</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="18" x14ac:dyDescent="0.3">
@@ -5537,11 +4365,11 @@
       </c>
       <c r="H47" s="22">
         <f>VLOOKUP(F47,SummaryReport!A:J,8,FALSE)</f>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I47" s="20">
         <f t="shared" si="20"/>
-        <v>-4.8951048951048959E-2</v>
+        <v>-3.3444816053511683E-3</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="18" x14ac:dyDescent="0.3">
@@ -5570,11 +4398,11 @@
       </c>
       <c r="H48" s="22">
         <f>VLOOKUP(F48,SummaryReport!A:J,8,FALSE)</f>
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I48" s="20">
         <f t="shared" si="20"/>
-        <v>5.177514792899518E-3</v>
+        <v>1.4652014652014711E-2</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="36" x14ac:dyDescent="0.3">
@@ -5747,8 +4575,8 @@
         <f>'Автоматизированный расчет'!A40</f>
         <v>Главная Welcome страница</v>
       </c>
-      <c r="B2" s="98" t="s">
-        <v>90</v>
+      <c r="B2" s="97" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -5756,7 +4584,7 @@
         <f>'Автоматизированный расчет'!A41</f>
         <v>Вход в систему</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="97" t="s">
         <v>24</v>
       </c>
     </row>
@@ -5765,8 +4593,8 @@
         <f>'Автоматизированный расчет'!A42</f>
         <v>Переход на страницу поиска билетов</v>
       </c>
-      <c r="B4" s="98" t="s">
-        <v>86</v>
+      <c r="B4" s="97" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -5774,8 +4602,8 @@
         <f>'Автоматизированный расчет'!A43</f>
         <v xml:space="preserve">Заполнение полей для поиска билета </v>
       </c>
-      <c r="B5" s="98" t="s">
-        <v>91</v>
+      <c r="B5" s="97" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -5783,8 +4611,8 @@
         <f>'Автоматизированный расчет'!A44</f>
         <v xml:space="preserve">Выбор рейса из найденных </v>
       </c>
-      <c r="B6" s="98" t="s">
-        <v>85</v>
+      <c r="B6" s="97" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -5792,8 +4620,8 @@
         <f>'Автоматизированный расчет'!A45</f>
         <v>Оплата билета</v>
       </c>
-      <c r="B7" s="98" t="s">
-        <v>92</v>
+      <c r="B7" s="97" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -5801,8 +4629,8 @@
         <f>'Автоматизированный расчет'!A46</f>
         <v>Просмотр квитанций</v>
       </c>
-      <c r="B8" s="98" t="s">
-        <v>88</v>
+      <c r="B8" s="97" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -5810,8 +4638,8 @@
         <f>'Автоматизированный расчет'!A47</f>
         <v xml:space="preserve">Отмена бронирования </v>
       </c>
-      <c r="B9" s="98" t="s">
-        <v>94</v>
+      <c r="B9" s="97" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -5819,7 +4647,7 @@
         <f>'Автоматизированный расчет'!A48</f>
         <v>Выход из системы</v>
       </c>
-      <c r="B10" s="98" t="s">
+      <c r="B10" s="97" t="s">
         <v>25</v>
       </c>
     </row>
@@ -5828,8 +4656,8 @@
         <f>'Автоматизированный расчет'!A49</f>
         <v>Перход на страницу регистрации</v>
       </c>
-      <c r="B11" s="98" t="s">
-        <v>89</v>
+      <c r="B11" s="97" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -5837,8 +4665,8 @@
         <f>'Автоматизированный расчет'!A50</f>
         <v>Заполнение полей регистарции</v>
       </c>
-      <c r="B12" s="98" t="s">
-        <v>93</v>
+      <c r="B12" s="97" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -5846,8 +4674,8 @@
         <f>'Автоматизированный расчет'!A51</f>
         <v>Переход на следуюущий эран после регистарции</v>
       </c>
-      <c r="B13" s="98" t="s">
-        <v>87</v>
+      <c r="B13" s="97" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -5873,8 +4701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5882,706 +4710,645 @@
     <col min="1" max="1" width="36.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="97" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="112" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="112" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="97" t="s">
+      <c r="C1" s="112" t="s">
         <v>75</v>
       </c>
-      <c r="D1" s="97" t="s">
+      <c r="D1" s="112" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="97" t="s">
+      <c r="E1" s="112" t="s">
         <v>77</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="112" t="s">
         <v>78</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="112" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="97" t="s">
+      <c r="H1" s="112" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="97" t="s">
+      <c r="I1" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="97" t="s">
+      <c r="J1" s="112" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="115" t="s">
-        <v>82</v>
-      </c>
-      <c r="B2" s="116" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="97" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="114">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="D2" s="114">
+        <v>0.32400000000000001</v>
+      </c>
+      <c r="E2" s="114">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="F2" s="114">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="G2" s="114">
+        <v>0.48699999999999999</v>
+      </c>
+      <c r="H2" s="114">
+        <v>88</v>
+      </c>
+      <c r="I2" s="114">
+        <v>0</v>
+      </c>
+      <c r="J2" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="97" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" s="114">
+        <v>0.46</v>
+      </c>
+      <c r="D3" s="114">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="E3" s="114">
+        <v>1.5209999999999999</v>
+      </c>
+      <c r="F3" s="114">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="G3" s="114">
+        <v>1.083</v>
+      </c>
+      <c r="H3" s="114">
+        <v>102</v>
+      </c>
+      <c r="I3" s="114">
+        <v>0</v>
+      </c>
+      <c r="J3" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="97" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="114">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D4" s="114">
+        <v>0.56799999999999995</v>
+      </c>
+      <c r="E4" s="114">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="F4" s="114">
+        <v>0.122</v>
+      </c>
+      <c r="G4" s="114">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="H4" s="114">
+        <v>31</v>
+      </c>
+      <c r="I4" s="114">
+        <v>0</v>
+      </c>
+      <c r="J4" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="97" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="114">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D5" s="114">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="E5" s="114">
+        <v>1.5449999999999999</v>
+      </c>
+      <c r="F5" s="114">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="G5" s="114">
+        <v>0.98</v>
+      </c>
+      <c r="H5" s="114">
+        <v>88</v>
+      </c>
+      <c r="I5" s="114">
+        <v>0</v>
+      </c>
+      <c r="J5" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="97" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="114">
+        <v>0.24</v>
+      </c>
+      <c r="D6" s="114">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="E6" s="114">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="F6" s="114">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G6" s="114">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="H6" s="114">
+        <v>31</v>
+      </c>
+      <c r="I6" s="114">
+        <v>0</v>
+      </c>
+      <c r="J6" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="114">
+        <v>0.46899999999999997</v>
+      </c>
+      <c r="D7" s="114">
+        <v>0.628</v>
+      </c>
+      <c r="E7" s="114">
+        <v>1.1060000000000001</v>
+      </c>
+      <c r="F7" s="114">
+        <v>0.157</v>
+      </c>
+      <c r="G7" s="114">
+        <v>0.877</v>
+      </c>
+      <c r="H7" s="114">
+        <v>186</v>
+      </c>
+      <c r="I7" s="114">
+        <v>0</v>
+      </c>
+      <c r="J7" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="97" t="s">
+        <v>90</v>
+      </c>
+      <c r="B8" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="114">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="D8" s="114">
+        <v>0.34</v>
+      </c>
+      <c r="E8" s="114">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="F8" s="114">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="G8" s="114">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="H8" s="114">
+        <v>88</v>
+      </c>
+      <c r="I8" s="114">
+        <v>4</v>
+      </c>
+      <c r="J8" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="97" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="114">
+        <v>0.496</v>
+      </c>
+      <c r="D9" s="114">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="E9" s="114">
+        <v>1.631</v>
+      </c>
+      <c r="F9" s="114">
+        <v>0.253</v>
+      </c>
+      <c r="G9" s="114">
+        <v>1.1479999999999999</v>
+      </c>
+      <c r="H9" s="114">
+        <v>155</v>
+      </c>
+      <c r="I9" s="114">
+        <v>0</v>
+      </c>
+      <c r="J9" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="97" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C10" s="114">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="D10" s="114">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="E10" s="114">
+        <v>0.92800000000000005</v>
+      </c>
+      <c r="F10" s="114">
+        <v>0.121</v>
+      </c>
+      <c r="G10" s="114">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="H10" s="114">
+        <v>105</v>
+      </c>
+      <c r="I10" s="114">
+        <v>0</v>
+      </c>
+      <c r="J10" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="97" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="114">
+        <v>0.252</v>
+      </c>
+      <c r="D11" s="114">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="E11" s="114">
+        <v>0.53700000000000003</v>
+      </c>
+      <c r="F11" s="114">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="G11" s="114">
+        <v>0.504</v>
+      </c>
+      <c r="H11" s="114">
+        <v>57</v>
+      </c>
+      <c r="I11" s="114">
+        <v>0</v>
+      </c>
+      <c r="J11" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="97" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C12" s="114">
+        <v>0.245</v>
+      </c>
+      <c r="D12" s="114">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="E12" s="114">
+        <v>0.58699999999999997</v>
+      </c>
+      <c r="F12" s="114">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G12" s="114">
+        <v>0.29899999999999999</v>
+      </c>
+      <c r="H12" s="114">
+        <v>31</v>
+      </c>
+      <c r="I12" s="114">
+        <v>0</v>
+      </c>
+      <c r="J12" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="B13" s="113" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="114">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="D13" s="114">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="E13" s="114">
+        <v>0.68600000000000005</v>
+      </c>
+      <c r="F13" s="114">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="G13" s="114">
+        <v>0.57599999999999996</v>
+      </c>
+      <c r="H13" s="114">
+        <v>23</v>
+      </c>
+      <c r="I13" s="114">
+        <v>0</v>
+      </c>
+      <c r="J13" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="B14" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="C14" s="114">
+        <v>1.9690000000000001</v>
+      </c>
+      <c r="D14" s="114">
+        <v>2.3250000000000002</v>
+      </c>
+      <c r="E14" s="114">
+        <v>3.45</v>
+      </c>
+      <c r="F14" s="114">
+        <v>0.314</v>
+      </c>
+      <c r="G14" s="114">
+        <v>2.617</v>
+      </c>
+      <c r="H14" s="114">
+        <v>30</v>
+      </c>
+      <c r="I14" s="114">
+        <v>0</v>
+      </c>
+      <c r="J14" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="114">
+        <v>1.994</v>
+      </c>
+      <c r="D15" s="114">
+        <v>2.5310000000000001</v>
+      </c>
+      <c r="E15" s="114">
+        <v>3.798</v>
+      </c>
+      <c r="F15" s="114">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="G15" s="114">
+        <v>3.3660000000000001</v>
+      </c>
+      <c r="H15" s="114">
+        <v>25</v>
+      </c>
+      <c r="I15" s="114">
+        <v>0</v>
+      </c>
+      <c r="J15" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="114">
+        <v>2.3759999999999999</v>
+      </c>
+      <c r="D16" s="114">
+        <v>2.8780000000000001</v>
+      </c>
+      <c r="E16" s="114">
+        <v>4.5129999999999999</v>
+      </c>
+      <c r="F16" s="114">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="G16" s="114">
+        <v>3.222</v>
+      </c>
+      <c r="H16" s="114">
+        <v>23</v>
+      </c>
+      <c r="I16" s="114">
+        <v>0</v>
+      </c>
+      <c r="J16" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="97" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="114">
+        <v>2.3380000000000001</v>
+      </c>
+      <c r="D17" s="114">
+        <v>3.0390000000000001</v>
+      </c>
+      <c r="E17" s="114">
+        <v>4.7709999999999999</v>
+      </c>
+      <c r="F17" s="114">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="G17" s="114">
+        <v>3.6869999999999998</v>
+      </c>
+      <c r="H17" s="114">
+        <v>34</v>
+      </c>
+      <c r="I17" s="114">
+        <v>4</v>
+      </c>
+      <c r="J17" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="113" t="s">
+        <v>99</v>
+      </c>
+      <c r="C18" s="114">
+        <v>3.012</v>
+      </c>
+      <c r="D18" s="114">
+        <v>4.1189999999999998</v>
+      </c>
+      <c r="E18" s="114">
+        <v>5.61</v>
+      </c>
+      <c r="F18" s="114">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="G18" s="114">
+        <v>4.8689999999999998</v>
+      </c>
+      <c r="H18" s="114">
+        <v>57</v>
+      </c>
+      <c r="I18" s="114">
+        <v>0</v>
+      </c>
+      <c r="J18" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="97" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="116">
-        <v>1.9690000000000001</v>
-      </c>
-      <c r="D2" s="116">
-        <v>3.1579999999999999</v>
-      </c>
-      <c r="E2" s="116">
-        <v>5.61</v>
-      </c>
-      <c r="F2" s="116">
-        <v>0.85899999999999999</v>
-      </c>
-      <c r="G2" s="116">
-        <v>4.3040000000000003</v>
-      </c>
-      <c r="H2" s="116">
-        <v>179</v>
-      </c>
-      <c r="I2" s="116">
-        <v>7</v>
-      </c>
-      <c r="J2" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="115" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="116">
-        <v>0.23300000000000001</v>
-      </c>
-      <c r="D3" s="116">
-        <v>0.32200000000000001</v>
-      </c>
-      <c r="E3" s="116">
-        <v>0.83299999999999996</v>
-      </c>
-      <c r="F3" s="116">
-        <v>9.7000000000000003E-2</v>
-      </c>
-      <c r="G3" s="116">
-        <v>0.46100000000000002</v>
-      </c>
-      <c r="H3" s="116">
-        <v>91</v>
-      </c>
-      <c r="I3" s="116">
-        <v>0</v>
-      </c>
-      <c r="J3" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="115" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C4" s="116">
-        <v>0.46</v>
-      </c>
-      <c r="D4" s="116">
-        <v>0.82199999999999995</v>
-      </c>
-      <c r="E4" s="116">
-        <v>1.5209999999999999</v>
-      </c>
-      <c r="F4" s="116">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="G4" s="116">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="H4" s="116">
-        <v>107</v>
-      </c>
-      <c r="I4" s="116">
-        <v>0</v>
-      </c>
-      <c r="J4" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="115" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C5" s="116">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="D5" s="116">
-        <v>0.55500000000000005</v>
-      </c>
-      <c r="E5" s="116">
-        <v>0.90600000000000003</v>
-      </c>
-      <c r="F5" s="116">
-        <v>0.11</v>
-      </c>
-      <c r="G5" s="116">
-        <v>0.71299999999999997</v>
-      </c>
-      <c r="H5" s="116">
-        <v>31</v>
-      </c>
-      <c r="I5" s="116">
-        <v>0</v>
-      </c>
-      <c r="J5" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="115" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="116">
-        <v>0.46600000000000003</v>
-      </c>
-      <c r="D6" s="116">
-        <v>0.66400000000000003</v>
-      </c>
-      <c r="E6" s="116">
-        <v>1.5449999999999999</v>
-      </c>
-      <c r="F6" s="116">
-        <v>0.21299999999999999</v>
-      </c>
-      <c r="G6" s="116">
-        <v>0.98</v>
-      </c>
-      <c r="H6" s="116">
-        <v>89</v>
-      </c>
-      <c r="I6" s="116">
-        <v>0</v>
-      </c>
-      <c r="J6" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="115" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C7" s="116">
-        <v>0.24</v>
-      </c>
-      <c r="D7" s="116">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="E7" s="116">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="F7" s="116">
-        <v>6.3E-2</v>
-      </c>
-      <c r="G7" s="116">
-        <v>0.373</v>
-      </c>
-      <c r="H7" s="116">
-        <v>31</v>
-      </c>
-      <c r="I7" s="116">
-        <v>0</v>
-      </c>
-      <c r="J7" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="115" t="s">
-        <v>90</v>
-      </c>
-      <c r="B8" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C8" s="116">
-        <v>0.46899999999999997</v>
-      </c>
-      <c r="D8" s="116">
-        <v>0.64600000000000002</v>
-      </c>
-      <c r="E8" s="116">
-        <v>1.3080000000000001</v>
-      </c>
-      <c r="F8" s="116">
-        <v>0.182</v>
-      </c>
-      <c r="G8" s="116">
-        <v>0.89100000000000001</v>
-      </c>
-      <c r="H8" s="116">
-        <v>187</v>
-      </c>
-      <c r="I8" s="116">
-        <v>0</v>
-      </c>
-      <c r="J8" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="115" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="116">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="D9" s="116">
-        <v>0.34100000000000003</v>
-      </c>
-      <c r="E9" s="116">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="F9" s="116">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="G9" s="116">
-        <v>0.53100000000000003</v>
-      </c>
-      <c r="H9" s="116">
-        <v>91</v>
-      </c>
-      <c r="I9" s="116">
-        <v>6</v>
-      </c>
-      <c r="J9" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="115" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="116">
-        <v>0.496</v>
-      </c>
-      <c r="D10" s="116">
-        <v>0.86599999999999999</v>
-      </c>
-      <c r="E10" s="116">
-        <v>2.6019999999999999</v>
-      </c>
-      <c r="F10" s="116">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="G10" s="116">
-        <v>1.375</v>
-      </c>
-      <c r="H10" s="116">
-        <v>155</v>
-      </c>
-      <c r="I10" s="116">
-        <v>0</v>
-      </c>
-      <c r="J10" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="115" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="116">
-        <v>0.44800000000000001</v>
-      </c>
-      <c r="D11" s="116">
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="E11" s="116">
-        <v>0.92800000000000005</v>
-      </c>
-      <c r="F11" s="116">
-        <v>0.122</v>
-      </c>
-      <c r="G11" s="116">
-        <v>0.78300000000000003</v>
-      </c>
-      <c r="H11" s="116">
-        <v>104</v>
-      </c>
-      <c r="I11" s="116">
-        <v>0</v>
-      </c>
-      <c r="J11" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="115" t="s">
-        <v>92</v>
-      </c>
-      <c r="B12" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="116">
-        <v>0.252</v>
-      </c>
-      <c r="D12" s="116">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="E12" s="116">
-        <v>0.53700000000000003</v>
-      </c>
-      <c r="F12" s="116">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="G12" s="116">
-        <v>0.504</v>
-      </c>
-      <c r="H12" s="116">
-        <v>57</v>
-      </c>
-      <c r="I12" s="116">
-        <v>0</v>
-      </c>
-      <c r="J12" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="115" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="116">
-        <v>0.245</v>
-      </c>
-      <c r="D13" s="116">
-        <v>0.27700000000000002</v>
-      </c>
-      <c r="E13" s="116">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="F13" s="116">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G13" s="116">
-        <v>0.29899999999999999</v>
-      </c>
-      <c r="H13" s="116">
-        <v>31</v>
-      </c>
-      <c r="I13" s="116">
-        <v>0</v>
-      </c>
-      <c r="J13" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="115" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="116">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="D14" s="116">
-        <v>0.45300000000000001</v>
-      </c>
-      <c r="E14" s="116">
-        <v>0.68600000000000005</v>
-      </c>
-      <c r="F14" s="116">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="G14" s="116">
-        <v>0.57599999999999996</v>
-      </c>
-      <c r="H14" s="116">
-        <v>22</v>
-      </c>
-      <c r="I14" s="116">
-        <v>1</v>
-      </c>
-      <c r="J14" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="115" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="116">
-        <v>1.9690000000000001</v>
-      </c>
-      <c r="D15" s="116">
-        <v>2.3340000000000001</v>
-      </c>
-      <c r="E15" s="116">
-        <v>3.45</v>
-      </c>
-      <c r="F15" s="116">
-        <v>0.312</v>
-      </c>
-      <c r="G15" s="116">
-        <v>2.617</v>
-      </c>
-      <c r="H15" s="116">
-        <v>31</v>
-      </c>
-      <c r="I15" s="116">
-        <v>0</v>
-      </c>
-      <c r="J15" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="115" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="C16" s="116">
-        <v>1.994</v>
-      </c>
-      <c r="D16" s="116">
-        <v>2.552</v>
-      </c>
-      <c r="E16" s="116">
-        <v>3.798</v>
-      </c>
-      <c r="F16" s="116">
-        <v>0.48599999999999999</v>
-      </c>
-      <c r="G16" s="116">
-        <v>3.3660000000000001</v>
-      </c>
-      <c r="H16" s="116">
-        <v>25</v>
-      </c>
-      <c r="I16" s="116">
-        <v>0</v>
-      </c>
-      <c r="J16" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="115" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="C17" s="116">
-        <v>2.3759999999999999</v>
-      </c>
-      <c r="D17" s="116">
-        <v>2.8730000000000002</v>
-      </c>
-      <c r="E17" s="116">
-        <v>4.5129999999999999</v>
-      </c>
-      <c r="F17" s="116">
-        <v>0.45900000000000002</v>
-      </c>
-      <c r="G17" s="116">
-        <v>3.222</v>
-      </c>
-      <c r="H17" s="116">
-        <v>22</v>
-      </c>
-      <c r="I17" s="116">
-        <v>1</v>
-      </c>
-      <c r="J17" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="115" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" s="116">
-        <v>2.3380000000000001</v>
-      </c>
-      <c r="D18" s="116">
-        <v>3.0390000000000001</v>
-      </c>
-      <c r="E18" s="116">
-        <v>4.7709999999999999</v>
-      </c>
-      <c r="F18" s="116">
-        <v>0.57099999999999995</v>
-      </c>
-      <c r="G18" s="116">
-        <v>3.6869999999999998</v>
-      </c>
-      <c r="H18" s="116">
-        <v>34</v>
-      </c>
-      <c r="I18" s="116">
-        <v>6</v>
-      </c>
-      <c r="J18" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="115" t="s">
+      <c r="B19" s="113" t="s">
         <v>99</v>
       </c>
-      <c r="B19" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="C19" s="116">
-        <v>3.012</v>
-      </c>
-      <c r="D19" s="116">
-        <v>4.1189999999999998</v>
-      </c>
-      <c r="E19" s="116">
-        <v>5.61</v>
-      </c>
-      <c r="F19" s="116">
-        <v>0.51400000000000001</v>
-      </c>
-      <c r="G19" s="116">
-        <v>4.8689999999999998</v>
-      </c>
-      <c r="H19" s="116">
-        <v>57</v>
-      </c>
-      <c r="I19" s="116">
-        <v>0</v>
-      </c>
-      <c r="J19" s="116">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="115" t="s">
-        <v>103</v>
-      </c>
-      <c r="B20" s="116" t="s">
-        <v>101</v>
-      </c>
-      <c r="C20" s="116">
+      <c r="C19" s="114">
         <v>2.0299999999999998</v>
       </c>
-      <c r="D20" s="116">
-        <v>2.778</v>
-      </c>
-      <c r="E20" s="116">
-        <v>4.8390000000000004</v>
-      </c>
-      <c r="F20" s="116">
-        <v>0.76400000000000001</v>
-      </c>
-      <c r="G20" s="116">
+      <c r="D19" s="114">
+        <v>2.5419999999999998</v>
+      </c>
+      <c r="E19" s="114">
         <v>3.1019999999999999</v>
       </c>
-      <c r="H20" s="116">
+      <c r="F19" s="114">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="G19" s="114">
+        <v>2.9420000000000002</v>
+      </c>
+      <c r="H19" s="113">
         <v>10</v>
       </c>
-      <c r="I20" s="116">
-        <v>0</v>
-      </c>
-      <c r="J20" s="116">
-        <v>0</v>
-      </c>
+      <c r="I19" s="114">
+        <v>0</v>
+      </c>
+      <c r="J19" s="114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="106"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="115" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" s="116" t="s">
-        <v>102</v>
-      </c>
-      <c r="C21" s="116">
-        <v>1E-3</v>
-      </c>
-      <c r="D21" s="116">
-        <v>3.0000000000000001E-3</v>
-      </c>
-      <c r="E21" s="116">
-        <v>1.6E-2</v>
-      </c>
-      <c r="F21" s="116">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G21" s="116">
-        <v>1.6E-2</v>
-      </c>
-      <c r="H21" s="116">
-        <v>9</v>
-      </c>
-      <c r="I21" s="116">
-        <v>0</v>
-      </c>
-      <c r="J21" s="116">
-        <v>0</v>
-      </c>
+      <c r="A21" s="106"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="117"/>
+      <c r="A22" s="106"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" xr:uid="{BF5F7FC7-A479-46F9-ACD3-72737B3FF748}"/>
-    <hyperlink ref="A3" xr:uid="{026E7AB1-FCEE-46D0-BF91-CC2D03D25AB9}"/>
-    <hyperlink ref="A4" xr:uid="{805757A6-C5DE-47B8-B14E-E214A0C68BD4}"/>
-    <hyperlink ref="A5" xr:uid="{414C6188-186F-4F07-8055-469348538AA7}"/>
-    <hyperlink ref="A6" xr:uid="{99036039-C5C9-4B4E-9C5A-8F60229B3AC4}"/>
-    <hyperlink ref="A7" xr:uid="{687C548C-0DCA-4E34-B4B8-8757A0196829}"/>
-    <hyperlink ref="A8" xr:uid="{8CAD1642-7A0E-41E4-9EBE-69B43ED36167}"/>
-    <hyperlink ref="A9" xr:uid="{176531E2-33A6-4C27-A2AC-1C4D1F1ACE83}"/>
-    <hyperlink ref="A10" xr:uid="{F30AE43E-4C33-4C32-B4FB-90082A4B6D48}"/>
-    <hyperlink ref="A11" xr:uid="{82D3AC57-A4D0-4183-8B2F-7B9266C6BA5A}"/>
-    <hyperlink ref="A12" xr:uid="{DA1D90D3-E61F-4BD1-BFA6-97D02AA8E6EA}"/>
-    <hyperlink ref="A13" xr:uid="{661BE65C-37B6-4FB5-981A-8A839105C98A}"/>
-    <hyperlink ref="A14" xr:uid="{311B304F-83D2-421E-B6FF-B3171FC96273}"/>
-    <hyperlink ref="A15" xr:uid="{FA4323CF-AABF-4744-BB67-8C21A9D9B79F}"/>
-    <hyperlink ref="A16" xr:uid="{3BDFC910-CC72-4647-A259-D2E68D9133E1}"/>
-    <hyperlink ref="A17" xr:uid="{44624376-BC5B-437A-8B82-9A2C70E3E329}"/>
-    <hyperlink ref="A18" xr:uid="{DD872862-541F-4476-9D6A-23C85F4160C5}"/>
-    <hyperlink ref="A19" xr:uid="{99B2DA88-2ADD-4D39-97BA-B622982E1FAD}"/>
-    <hyperlink ref="A20" xr:uid="{E71F4B8B-9DEF-4255-A071-65121D44E2E2}"/>
-    <hyperlink ref="A21" xr:uid="{AC94B147-5636-4A18-8F92-BB5D2739E571}"/>
+    <hyperlink ref="A2" xr:uid="{1A2D7DFA-87BB-42B9-ABFA-6BACBB5C02D5}"/>
+    <hyperlink ref="A3" xr:uid="{B2E5DEFF-90B8-4977-AFDE-5D7F9B4C3356}"/>
+    <hyperlink ref="A4" xr:uid="{668ABCB5-D5C9-4DB2-A1F4-CEB6A3DD78D0}"/>
+    <hyperlink ref="A5" xr:uid="{AE7584C7-88D4-4D98-8392-FCC9F5689AE5}"/>
+    <hyperlink ref="A6" xr:uid="{5FE40E51-9D1E-44A7-9671-9514C111D8C7}"/>
+    <hyperlink ref="A7" xr:uid="{AABA0309-10A0-469D-889D-36328867D41D}"/>
+    <hyperlink ref="A8" xr:uid="{38E6A321-8944-4655-AE29-A41440ABB56B}"/>
+    <hyperlink ref="A9" xr:uid="{A1988DA0-742C-47C4-8591-0E44D754F96B}"/>
+    <hyperlink ref="A10" xr:uid="{DF91D120-E7AD-418B-8352-00C658B1CA26}"/>
+    <hyperlink ref="A11" xr:uid="{F65D6814-60CE-4A6E-9A2F-F0CB06C90CD2}"/>
+    <hyperlink ref="A12" xr:uid="{80D30D61-21EE-464D-A48F-629698591DE4}"/>
+    <hyperlink ref="A13" xr:uid="{213A7945-2AFA-4DC7-8B59-57775DB07BB3}"/>
+    <hyperlink ref="A14" xr:uid="{68DBDB7C-6104-4939-8923-31F2EBDF8401}"/>
+    <hyperlink ref="A15" xr:uid="{08D15DA6-6AC2-4660-8979-0C91045A0077}"/>
+    <hyperlink ref="A16" xr:uid="{ABCE5691-940D-4014-B9B8-DBC7F4425BB1}"/>
+    <hyperlink ref="A17" xr:uid="{615F7BB5-D6FA-4371-8AB1-BB736AEB0B9A}"/>
+    <hyperlink ref="A18" xr:uid="{D706BAE4-68E1-4FCC-A401-02E18B946686}"/>
+    <hyperlink ref="A19" xr:uid="{1FEE22C1-7CA4-43F2-BD62-7EB40247BAF6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6612,13 +5379,13 @@
   </cols>
   <sheetData>
     <row r="9" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E9" s="103" t="s">
+      <c r="E9" s="111" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="103"/>
-      <c r="G9" s="103"/>
-      <c r="H9" s="103"/>
-      <c r="I9" s="103"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="111"/>
     </row>
     <row r="11" spans="5:9" ht="27.6" x14ac:dyDescent="0.3">
       <c r="E11" s="1" t="s">
@@ -6771,13 +5538,13 @@
       </c>
     </row>
     <row r="23" spans="5:9" x14ac:dyDescent="0.3">
-      <c r="E23" s="103" t="s">
+      <c r="E23" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="103"/>
+      <c r="F23" s="111"/>
+      <c r="G23" s="111"/>
+      <c r="H23" s="111"/>
+      <c r="I23" s="111"/>
     </row>
     <row r="25" spans="5:9" x14ac:dyDescent="0.3">
       <c r="E25" s="8" t="s">
@@ -6937,13 +5704,13 @@
       </c>
     </row>
     <row r="35" spans="5:15" x14ac:dyDescent="0.3">
-      <c r="E35" s="103" t="s">
+      <c r="E35" s="111" t="s">
         <v>32</v>
       </c>
-      <c r="F35" s="103"/>
-      <c r="G35" s="103"/>
-      <c r="H35" s="103"/>
-      <c r="I35" s="103"/>
+      <c r="F35" s="111"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="111"/>
+      <c r="I35" s="111"/>
     </row>
     <row r="37" spans="5:15" x14ac:dyDescent="0.3">
       <c r="E37" s="8" t="s">

</xml_diff>